<commit_message>
major changes, function and analyses
</commit_message>
<xml_diff>
--- a/biomass_data_matinha_USP.xlsx
+++ b/biomass_data_matinha_USP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro M\Desktop\r_analizes\palms_biomass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F95C4C-CB1E-4FEC-A92C-1C1A1885E43E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2E2EF6-4B50-4A75-8D6D-FA127E33C624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F188378-987B-47FF-A329-9F0565C0E1BF}"/>
   </bookViews>
@@ -475,8 +475,8 @@
   <dimension ref="A1:J828"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A794" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C825" sqref="C825"/>
+      <pane ySplit="1" topLeftCell="A795" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X811" sqref="X811"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12739,6 +12739,13 @@
       <c r="F525">
         <v>1000</v>
       </c>
+      <c r="G525">
+        <v>238</v>
+      </c>
+      <c r="H525">
+        <f>(G525*100/F525)/100</f>
+        <v>0.23800000000000002</v>
+      </c>
       <c r="I525" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
model linear and plot
</commit_message>
<xml_diff>
--- a/biomass_data_matinha_USP.xlsx
+++ b/biomass_data_matinha_USP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro M\Desktop\r_analizes\palms_biomass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E742CF7D-C01F-4725-9596-7894BDEDE2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F3545C-72C9-41DE-A2EF-D8DAFDC2394C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F188378-987B-47FF-A329-9F0565C0E1BF}"/>
   </bookViews>
@@ -490,8 +490,8 @@
   <dimension ref="A1:J1877"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1854" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1860" sqref="J1860:J1877"/>
+      <pane ySplit="1" topLeftCell="A330" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1331" sqref="E1331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31454,7 +31454,7 @@
         <v>27.89</v>
       </c>
       <c r="E1331">
-        <v>229</v>
+        <v>29</v>
       </c>
       <c r="F1331">
         <v>190</v>

</xml_diff>